<commit_message>
Fixed helper, made generated model with ROC analysis
</commit_message>
<xml_diff>
--- a/zipfCheck/TestResults.xlsx
+++ b/zipfCheck/TestResults.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filestore.soton.ac.uk\users\ac19g14\mydocuments\Year 4\ML\zipfCheck\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ECS WORK FOLDERS\Year 4\COMP62something - Adv Machine Learning\project\zipfCheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -298,7 +298,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B9D9-4C55-B4FC-BB61A0C8F11A}"/>
             </c:ext>
@@ -437,7 +437,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B9D9-4C55-B4FC-BB61A0C8F11A}"/>
             </c:ext>
@@ -451,11 +451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2090038832"/>
-        <c:axId val="2090034672"/>
+        <c:axId val="472586976"/>
+        <c:axId val="472592856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2090038832"/>
+        <c:axId val="472586976"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -513,12 +513,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090034672"/>
+        <c:crossAx val="472592856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090034672"/>
+        <c:axId val="472592856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090038832"/>
+        <c:crossAx val="472586976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -657,7 +657,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -826,7 +826,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-935C-46EB-B03D-49E27AB06943}"/>
             </c:ext>
@@ -941,7 +941,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-935C-46EB-B03D-49E27AB06943}"/>
             </c:ext>
@@ -955,11 +955,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2090038832"/>
-        <c:axId val="2090034672"/>
+        <c:axId val="472588544"/>
+        <c:axId val="184506040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2090038832"/>
+        <c:axId val="472588544"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1017,12 +1017,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090034672"/>
+        <c:crossAx val="184506040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090034672"/>
+        <c:axId val="184506040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090038832"/>
+        <c:crossAx val="472588544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1699,15 +1699,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1729,15 +1729,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2027,7 +2027,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>